<commit_message>
Nova funcao produtos_existentes e alterada a funcao atualizar_base_resultados para permitir atualizar todas as bases
</commit_message>
<xml_diff>
--- a/data-raw/resultados_supersete.xlsx
+++ b/data-raw/resultados_supersete.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2052"/>
+  <dimension ref="A1:E2059"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -35258,6 +35258,125 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2053">
+      <c r="A2053" s="2">
+        <v>44816</v>
+      </c>
+      <c r="B2053">
+        <v>294</v>
+      </c>
+      <c r="C2053">
+        <v>0</v>
+      </c>
+      <c r="D2053">
+        <v>0</v>
+      </c>
+      <c r="E2053">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2054">
+      <c r="A2054" s="2">
+        <v>44816</v>
+      </c>
+      <c r="B2054">
+        <v>294</v>
+      </c>
+      <c r="C2054">
+        <v>0</v>
+      </c>
+      <c r="D2054">
+        <v>0</v>
+      </c>
+      <c r="E2054">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2055">
+      <c r="A2055" s="2">
+        <v>44816</v>
+      </c>
+      <c r="B2055">
+        <v>294</v>
+      </c>
+      <c r="C2055">
+        <v>0</v>
+      </c>
+      <c r="D2055">
+        <v>0</v>
+      </c>
+      <c r="E2055">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2056">
+      <c r="A2056" s="2">
+        <v>44816</v>
+      </c>
+      <c r="B2056">
+        <v>294</v>
+      </c>
+      <c r="C2056">
+        <v>0</v>
+      </c>
+      <c r="D2056">
+        <v>0</v>
+      </c>
+      <c r="E2056">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2057">
+      <c r="A2057" s="2">
+        <v>44816</v>
+      </c>
+      <c r="B2057">
+        <v>294</v>
+      </c>
+      <c r="C2057">
+        <v>0</v>
+      </c>
+      <c r="D2057">
+        <v>0</v>
+      </c>
+      <c r="E2057">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2058">
+      <c r="A2058" s="2">
+        <v>44816</v>
+      </c>
+      <c r="B2058">
+        <v>294</v>
+      </c>
+      <c r="C2058">
+        <v>0</v>
+      </c>
+      <c r="D2058">
+        <v>0</v>
+      </c>
+      <c r="E2058">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2059">
+      <c r="A2059" s="2">
+        <v>44816</v>
+      </c>
+      <c r="B2059">
+        <v>294</v>
+      </c>
+      <c r="C2059">
+        <v>0</v>
+      </c>
+      <c r="D2059">
+        <v>0</v>
+      </c>
+      <c r="E2059">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>